<commit_message>
update account value 2. bottom shape when the top is not reached.
</commit_message>
<xml_diff>
--- a/projection.xlsx
+++ b/projection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggao\Documents\mynote\gegaoty.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0D5B2D-67A3-4B7B-97ED-89537147DA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A60BD1-BA1A-4748-9D26-C8C28CFD03F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82DD70FC-F872-4E7F-9B20-671305A83F30}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{82DD70FC-F872-4E7F-9B20-671305A83F30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1464,23 +1464,23 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="A10" sqref="A10:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="10" width="10.85546875" customWidth="1"/>
+    <col min="9" max="10" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>13</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -1520,8 +1520,8 @@
         <v>47100</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1551,9 +1551,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+        <f t="shared" ref="A8:A29" si="0">$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
         <v>2021</v>
       </c>
       <c r="B8" t="str">
@@ -1569,7 +1569,7 @@
         <v>47.1</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E29" si="0">INT(C8/$E$2)</f>
+        <f t="shared" ref="E8:E29" si="1">INT(C8/$E$2)</f>
         <v>1</v>
       </c>
       <c r="F8">
@@ -1592,351 +1592,357 @@
         <v>47100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+        <f t="shared" si="0"/>
         <v>2021</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" ref="B9:B17" si="1">TEXT((ROW()-ROW($B$8)+$E$4)*29,"mmm")</f>
+        <f t="shared" ref="B9:B17" si="2">TEXT((ROW()-ROW($B$8)+$E$4)*29,"mmm")</f>
         <v>Apr</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C29" si="2">C8+F8</f>
+        <f t="shared" ref="C9:C29" si="3">C8+F8</f>
         <v>62100</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D27" si="3">C9/1000</f>
+        <f t="shared" ref="D9:D27" si="4">C9/1000</f>
         <v>62.1</v>
       </c>
       <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F29" si="5">E9*$E$1*50</f>
+        <v>15000</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G29" si="6">F9/1000</f>
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H29" si="7">D9/1000</f>
+        <v>6.2100000000000002E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I29" si="8">INT(1000*F9/C9)/10</f>
+        <v>24.1</v>
+      </c>
+      <c r="J9">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
         <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="2"/>
+        <v>May</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
+        <v>77100</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="4"/>
+        <v>77.099999999999994</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F29" si="4">E9*$E$1*50</f>
+      <c r="F10">
+        <f t="shared" si="5"/>
         <v>15000</v>
       </c>
-      <c r="G9">
-        <f t="shared" ref="G9:G29" si="5">F9/1000</f>
+      <c r="G10">
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="H9">
-        <f t="shared" ref="H9:H29" si="6">D9/1000</f>
-        <v>6.2100000000000002E-2</v>
-      </c>
-      <c r="I9">
-        <f t="shared" ref="I9:I29" si="7">INT(1000*F9/C9)/10</f>
-        <v>24.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+      <c r="H10">
+        <f t="shared" si="7"/>
+        <v>7.7099999999999988E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="8"/>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="J10">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B11" t="str">
+        <f t="shared" si="2"/>
+        <v>Jun</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>92100</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="4"/>
+        <v>92.1</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="1"/>
-        <v>May</v>
-      </c>
-      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="5"/>
+        <v>30000</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="7"/>
+        <v>9.2099999999999987E-2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="8"/>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="B12" t="str">
         <f t="shared" si="2"/>
-        <v>77100</v>
-      </c>
-      <c r="D10">
+        <v>Jul</v>
+      </c>
+      <c r="C12">
         <f t="shared" si="3"/>
-        <v>77.099999999999994</v>
-      </c>
-      <c r="E10">
+        <v>122100</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>122.1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="5"/>
+        <v>45000</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="7"/>
+        <v>0.1221</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="8"/>
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F10">
+        <v>2021</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="2"/>
+        <v>Aug</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="3"/>
+        <v>167100</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="4"/>
-        <v>15000</v>
-      </c>
-      <c r="G10">
+        <v>167.1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="H10">
+        <v>60000</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="6"/>
-        <v>7.7099999999999988E-2</v>
-      </c>
-      <c r="I10">
+        <v>60</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="7"/>
-        <v>19.399999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+        <v>0.1671</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="8"/>
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B14" t="str">
+        <f t="shared" si="2"/>
+        <v>Sep</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>227100</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="4"/>
+        <v>227.1</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="1"/>
-        <v>Jun</v>
-      </c>
-      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="5"/>
+        <v>75000</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="6"/>
+        <v>75</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="7"/>
+        <v>0.2271</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="8"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="B15" t="str">
         <f t="shared" si="2"/>
-        <v>92100</v>
-      </c>
-      <c r="D11">
+        <v>Oct</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="3"/>
-        <v>92.1</v>
-      </c>
-      <c r="E11">
+        <v>302100</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="4"/>
+        <v>302.10000000000002</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="5"/>
+        <v>105000</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="6"/>
+        <v>105</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="7"/>
+        <v>0.30210000000000004</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="8"/>
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F11">
+        <v>2021</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="2"/>
+        <v>Nov</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>407100</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="4"/>
-        <v>30000</v>
-      </c>
-      <c r="G11">
+        <v>407.1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="H11">
+        <v>150000</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="6"/>
-        <v>9.2099999999999987E-2</v>
-      </c>
-      <c r="I11">
+        <v>150</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="7"/>
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+        <v>0.40710000000000002</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="8"/>
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B17" t="str">
+        <f t="shared" si="2"/>
+        <v>Dec</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="3"/>
+        <v>557100</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>557.1</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="1"/>
-        <v>Jul</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="2"/>
-        <v>122100</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="3"/>
-        <v>122.1</v>
-      </c>
-      <c r="E12">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="5"/>
+        <v>195000</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="6"/>
+        <v>195</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="7"/>
+        <v>0.55710000000000004</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="4"/>
-        <v>45000</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="5"/>
-        <v>45</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="6"/>
-        <v>0.1221</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="7"/>
-        <v>36.799999999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2021</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="1"/>
-        <v>Aug</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="2"/>
-        <v>167100</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="3"/>
-        <v>167.1</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="4"/>
-        <v>60000</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="5"/>
-        <v>60</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="6"/>
-        <v>0.1671</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="7"/>
-        <v>35.9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2021</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="1"/>
-        <v>Sep</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="2"/>
-        <v>227100</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="3"/>
-        <v>227.1</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="4"/>
-        <v>75000</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="5"/>
-        <v>75</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="6"/>
-        <v>0.2271</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="7"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2021</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="1"/>
-        <v>Oct</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="2"/>
-        <v>302100</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="3"/>
-        <v>302.10000000000002</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="4"/>
-        <v>105000</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="5"/>
-        <v>105</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="6"/>
-        <v>0.30210000000000004</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="7"/>
-        <v>34.700000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2021</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" si="1"/>
-        <v>Nov</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="2"/>
-        <v>407100</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="3"/>
-        <v>407.1</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="4"/>
-        <v>150000</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="5"/>
-        <v>150</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="6"/>
-        <v>0.40710000000000002</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="7"/>
-        <v>36.799999999999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2021</v>
-      </c>
-      <c r="B17" t="str">
-        <f t="shared" si="1"/>
-        <v>Dec</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="2"/>
-        <v>557100</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="3"/>
-        <v>557.1</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="4"/>
-        <v>195000</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="5"/>
-        <v>195</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="6"/>
-        <v>0.55710000000000004</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="7"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
         <v>2022</v>
       </c>
       <c r="B18" t="str">
@@ -1944,449 +1950,449 @@
         <v>Jan</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>752100</v>
       </c>
       <c r="D18">
+        <f t="shared" si="4"/>
+        <v>752.1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>270000</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="6"/>
+        <v>270</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="7"/>
+        <v>0.75209999999999999</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="8"/>
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" ref="B19:B29" si="9">TEXT((ROW()-ROW($B$8)+$E$4)*29,"mmm")</f>
+        <v>Feb</v>
+      </c>
+      <c r="C19">
         <f t="shared" si="3"/>
-        <v>752.1</v>
-      </c>
-      <c r="E18">
+        <v>1022100</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="4"/>
+        <v>1022.1</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="5"/>
+        <v>375000</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="6"/>
+        <v>375</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="7"/>
+        <v>1.0221</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="8"/>
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="F18">
+        <v>2022</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="9"/>
+        <v>Mar</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="3"/>
+        <v>1397100</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="4"/>
-        <v>270000</v>
-      </c>
-      <c r="G18">
+        <v>1397.1</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="F20">
         <f t="shared" si="5"/>
-        <v>270</v>
-      </c>
-      <c r="H18">
+        <v>510000</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="6"/>
-        <v>0.75209999999999999</v>
-      </c>
-      <c r="I18">
+        <v>510</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="7"/>
-        <v>35.799999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+        <v>1.3971</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="8"/>
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="B19" t="str">
-        <f t="shared" ref="B19:B29" si="8">TEXT((ROW()-ROW($B$8)+$E$4)*29,"mmm")</f>
-        <v>Feb</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="2"/>
-        <v>1022100</v>
-      </c>
-      <c r="D19">
+      <c r="B21" t="str">
+        <f t="shared" si="9"/>
+        <v>Apr</v>
+      </c>
+      <c r="C21">
         <f t="shared" si="3"/>
-        <v>1022.1</v>
-      </c>
-      <c r="E19">
+        <v>1907100</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="4"/>
+        <v>1907.1</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>705000</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="6"/>
+        <v>705</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
+        <v>1.9071</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="8"/>
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="F19">
+        <v>2022</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="9"/>
+        <v>May</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="3"/>
+        <v>2612100</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="4"/>
-        <v>375000</v>
-      </c>
-      <c r="G19">
+        <v>2612.1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="F22">
         <f t="shared" si="5"/>
-        <v>375</v>
-      </c>
-      <c r="H19">
+        <v>975000</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="6"/>
-        <v>1.0221</v>
-      </c>
-      <c r="I19">
+        <v>975</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="7"/>
-        <v>36.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+        <v>2.6120999999999999</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="8"/>
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B23" t="str">
+        <f t="shared" si="9"/>
+        <v>Jun</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>3587100</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="4"/>
+        <v>3587.1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>1335000</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="6"/>
+        <v>1335</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="7"/>
+        <v>3.5871</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="8"/>
-        <v>Mar</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="2"/>
-        <v>1397100</v>
-      </c>
-      <c r="D20">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="9"/>
+        <v>Jul</v>
+      </c>
+      <c r="C24">
         <f t="shared" si="3"/>
-        <v>1397.1</v>
-      </c>
-      <c r="E20">
+        <v>4922100</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="4"/>
+        <v>4922.1000000000004</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="5"/>
+        <v>1845000</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="6"/>
+        <v>1845</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="7"/>
+        <v>4.9221000000000004</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="8"/>
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25">
         <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="F20">
+        <v>2022</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="9"/>
+        <v>Aug</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>6767100</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="4"/>
-        <v>510000</v>
-      </c>
-      <c r="G20">
+        <v>6767.1</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>169</v>
+      </c>
+      <c r="F25">
         <f t="shared" si="5"/>
-        <v>510</v>
-      </c>
-      <c r="H20">
+        <v>2535000</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="6"/>
-        <v>1.3971</v>
-      </c>
-      <c r="I20">
+        <v>2535</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="7"/>
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+        <v>6.7671000000000001</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="8"/>
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B26" t="str">
+        <f t="shared" si="9"/>
+        <v>Aug</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>9302100</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="4"/>
+        <v>9302.1</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>232</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="5"/>
+        <v>3480000</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="6"/>
+        <v>3480</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="7"/>
+        <v>9.3021000000000011</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="8"/>
-        <v>Apr</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
-        <v>1907100</v>
-      </c>
-      <c r="D21">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="9"/>
+        <v>Sep</v>
+      </c>
+      <c r="C27">
         <f t="shared" si="3"/>
-        <v>1907.1</v>
-      </c>
-      <c r="E21">
+        <v>12782100</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="4"/>
+        <v>12782.1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>319</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="5"/>
+        <v>4785000</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="6"/>
+        <v>4785</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="7"/>
+        <v>12.7821</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="8"/>
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="4"/>
-        <v>705000</v>
-      </c>
-      <c r="G21">
+        <v>2022</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="9"/>
+        <v>Oct</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="3"/>
+        <v>17567100</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:D29" si="10">C28/1000</f>
+        <v>17567.099999999999</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>439</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="5"/>
-        <v>705</v>
-      </c>
-      <c r="H21">
+        <v>6585000</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="6"/>
-        <v>1.9071</v>
-      </c>
-      <c r="I21">
+        <v>6585</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="7"/>
-        <v>36.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
+        <v>17.5671</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="8"/>
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B29" t="str">
+        <f t="shared" si="9"/>
+        <v>Nov</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="3"/>
+        <v>24152100</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="10"/>
+        <v>24152.1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>603</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>9045000</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="6"/>
+        <v>9045</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="7"/>
+        <v>24.152099999999997</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="8"/>
-        <v>May</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="2"/>
-        <v>2612100</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="3"/>
-        <v>2612.1</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="4"/>
-        <v>975000</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="5"/>
-        <v>975</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="6"/>
-        <v>2.6120999999999999</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="7"/>
-        <v>37.299999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2022</v>
-      </c>
-      <c r="B23" t="str">
-        <f t="shared" si="8"/>
-        <v>Jun</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="2"/>
-        <v>3587100</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="3"/>
-        <v>3587.1</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="4"/>
-        <v>1335000</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="5"/>
-        <v>1335</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="6"/>
-        <v>3.5871</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="7"/>
-        <v>37.200000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2022</v>
-      </c>
-      <c r="B24" t="str">
-        <f t="shared" si="8"/>
-        <v>Jul</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="2"/>
-        <v>4922100</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="3"/>
-        <v>4922.1000000000004</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>123</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="4"/>
-        <v>1845000</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="5"/>
-        <v>1845</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="6"/>
-        <v>4.9221000000000004</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="7"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2022</v>
-      </c>
-      <c r="B25" t="str">
-        <f t="shared" si="8"/>
-        <v>Aug</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="2"/>
-        <v>6767100</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="3"/>
-        <v>6767.1</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>169</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="4"/>
-        <v>2535000</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="5"/>
-        <v>2535</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="6"/>
-        <v>6.7671000000000001</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="7"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2022</v>
-      </c>
-      <c r="B26" t="str">
-        <f t="shared" si="8"/>
-        <v>Aug</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="2"/>
-        <v>9302100</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="3"/>
-        <v>9302.1</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>232</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="4"/>
-        <v>3480000</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="5"/>
-        <v>3480</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="6"/>
-        <v>9.3021000000000011</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="7"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2022</v>
-      </c>
-      <c r="B27" t="str">
-        <f t="shared" si="8"/>
-        <v>Sep</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="2"/>
-        <v>12782100</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="3"/>
-        <v>12782.1</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>319</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="4"/>
-        <v>4785000</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="5"/>
-        <v>4785</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="6"/>
-        <v>12.7821</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="7"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2022</v>
-      </c>
-      <c r="B28" t="str">
-        <f t="shared" si="8"/>
-        <v>Oct</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="2"/>
-        <v>17567100</v>
-      </c>
-      <c r="D28">
-        <f t="shared" ref="D28:D29" si="9">C28/1000</f>
-        <v>17567.099999999999</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>439</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="4"/>
-        <v>6585000</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="5"/>
-        <v>6585</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="6"/>
-        <v>17.5671</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="7"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f>$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2022</v>
-      </c>
-      <c r="B29" t="str">
-        <f t="shared" si="8"/>
-        <v>Nov</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="2"/>
-        <v>24152100</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="9"/>
-        <v>24152.1</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>603</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="4"/>
-        <v>9045000</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="5"/>
-        <v>9045</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="6"/>
-        <v>24.152099999999997</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="7"/>
         <v>37.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add more one note.
</commit_message>
<xml_diff>
--- a/projection.xlsx
+++ b/projection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggao\Documents\mynote\gegaoty.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A60BD1-BA1A-4748-9D26-C8C28CFD03F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9970E7-3C16-4C84-A1AB-E4AC76520C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{82DD70FC-F872-4E7F-9B20-671305A83F30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82DD70FC-F872-4E7F-9B20-671305A83F30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1464,7 +1464,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:J10"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1711,6 +1711,9 @@
         <f t="shared" si="8"/>
         <v>32.5</v>
       </c>
+      <c r="J11">
+        <v>24000</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1748,6 +1751,9 @@
       <c r="I12">
         <f t="shared" si="8"/>
         <v>36.799999999999997</v>
+      </c>
+      <c r="J12">
+        <v>8000</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update to new mode. 1. middle relative weak mode. 2. rebound Hard during retreat of bull market.
</commit_message>
<xml_diff>
--- a/projection.xlsx
+++ b/projection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggao\Documents\mynote\gegaoty.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9970E7-3C16-4C84-A1AB-E4AC76520C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9131F35D-C24E-404A-9E5A-84AE1E640FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82DD70FC-F872-4E7F-9B20-671305A83F30}"/>
   </bookViews>
@@ -288,40 +288,40 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Mar</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>Apr</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>May</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>Jun</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>Jul</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>Aug</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>Sep</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>Oct</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>Nov</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>Dec</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Feb</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -333,40 +333,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>47100</c:v>
+                  <c:v>47000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62100</c:v>
+                  <c:v>57000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77100</c:v>
+                  <c:v>67000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92100</c:v>
+                  <c:v>77000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122100</c:v>
+                  <c:v>87000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>167100</c:v>
+                  <c:v>107000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>227100</c:v>
+                  <c:v>127000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>302100</c:v>
+                  <c:v>157000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>407100</c:v>
+                  <c:v>187000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>557100</c:v>
+                  <c:v>227000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>752100</c:v>
+                  <c:v>277000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1022100</c:v>
+                  <c:v>337000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1464,31 +1464,31 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="10" width="10.88671875" customWidth="1"/>
+    <col min="9" max="10" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1496,32 +1496,32 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="1">
-        <v>47100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>47000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1551,22 +1551,22 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ref="A8:A29" si="0">$E$3+INT((ROW()-ROW($A$8)+$E$4-1)/12)</f>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B8" t="str">
         <f>TEXT((ROW()-ROW($B$8)+$E$4)*29,"mmm")</f>
-        <v>Mar</v>
+        <v>Jan</v>
       </c>
       <c r="C8">
         <f>E5</f>
-        <v>47100</v>
+        <v>47000</v>
       </c>
       <c r="D8">
         <f>C8/1000</f>
-        <v>47.1</v>
+        <v>47</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:E29" si="1">INT(C8/$E$2)</f>
@@ -1574,40 +1574,40 @@
       </c>
       <c r="F8">
         <f>E8*$E$1*50</f>
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="G8">
         <f>F8/1000</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H8">
         <f>D8/1000</f>
-        <v>4.7100000000000003E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="I8">
         <f>INT(1000*F8/C8)/10</f>
-        <v>31.8</v>
+        <v>21.2</v>
       </c>
       <c r="J8">
         <v>47100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" ref="B9:B17" si="2">TEXT((ROW()-ROW($B$8)+$E$4)*29,"mmm")</f>
-        <v>Apr</v>
+        <v>Feb</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C29" si="3">C8+F8</f>
-        <v>62100</v>
+        <v>57000</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9:D27" si="4">C9/1000</f>
-        <v>62.1</v>
+        <v>57</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
@@ -1615,40 +1615,40 @@
       </c>
       <c r="F9">
         <f t="shared" ref="F9:F29" si="5">E9*$E$1*50</f>
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="G9">
         <f t="shared" ref="G9:G29" si="6">F9/1000</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H9">
         <f t="shared" ref="H9:H29" si="7">D9/1000</f>
-        <v>6.2100000000000002E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="I9">
         <f t="shared" ref="I9:I29" si="8">INT(1000*F9/C9)/10</f>
-        <v>24.1</v>
+        <v>17.5</v>
       </c>
       <c r="J9">
         <v>55000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="2"/>
-        <v>May</v>
+        <v>Mar</v>
       </c>
       <c r="C10">
         <f t="shared" si="3"/>
-        <v>77100</v>
+        <v>67000</v>
       </c>
       <c r="D10">
         <f t="shared" si="4"/>
-        <v>77.099999999999994</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
@@ -1656,750 +1656,750 @@
       </c>
       <c r="F10">
         <f t="shared" si="5"/>
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="G10">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H10">
         <f t="shared" si="7"/>
-        <v>7.7099999999999988E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="I10">
         <f t="shared" si="8"/>
-        <v>19.399999999999999</v>
+        <v>14.9</v>
       </c>
       <c r="J10">
         <v>25000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="2"/>
-        <v>Jun</v>
+        <v>Apr</v>
       </c>
       <c r="C11">
         <f t="shared" si="3"/>
-        <v>92100</v>
+        <v>77000</v>
       </c>
       <c r="D11">
         <f t="shared" si="4"/>
-        <v>92.1</v>
+        <v>77</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" si="5"/>
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="G11">
         <f t="shared" si="6"/>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <f t="shared" si="7"/>
-        <v>9.2099999999999987E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="I11">
         <f t="shared" si="8"/>
-        <v>32.5</v>
+        <v>12.9</v>
       </c>
       <c r="J11">
         <v>24000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="2"/>
-        <v>Jul</v>
+        <v>May</v>
       </c>
       <c r="C12">
         <f t="shared" si="3"/>
-        <v>122100</v>
+        <v>87000</v>
       </c>
       <c r="D12">
         <f t="shared" si="4"/>
-        <v>122.1</v>
+        <v>87</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <f t="shared" si="5"/>
-        <v>45000</v>
+        <v>20000</v>
       </c>
       <c r="G12">
         <f t="shared" si="6"/>
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="H12">
         <f t="shared" si="7"/>
-        <v>0.1221</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="I12">
         <f t="shared" si="8"/>
-        <v>36.799999999999997</v>
+        <v>22.9</v>
       </c>
       <c r="J12">
         <v>8000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="2"/>
-        <v>Aug</v>
+        <v>Jun</v>
       </c>
       <c r="C13">
         <f t="shared" si="3"/>
-        <v>167100</v>
+        <v>107000</v>
       </c>
       <c r="D13">
         <f t="shared" si="4"/>
-        <v>167.1</v>
+        <v>107</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F13">
         <f t="shared" si="5"/>
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="G13">
         <f t="shared" si="6"/>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="H13">
         <f t="shared" si="7"/>
-        <v>0.1671</v>
+        <v>0.107</v>
       </c>
       <c r="I13">
         <f t="shared" si="8"/>
-        <v>35.9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="2"/>
-        <v>Sep</v>
+        <v>Jul</v>
       </c>
       <c r="C14">
         <f t="shared" si="3"/>
-        <v>227100</v>
+        <v>127000</v>
       </c>
       <c r="D14">
         <f t="shared" si="4"/>
-        <v>227.1</v>
+        <v>127</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14">
         <f t="shared" si="5"/>
-        <v>75000</v>
+        <v>30000</v>
       </c>
       <c r="G14">
         <f t="shared" si="6"/>
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="H14">
         <f t="shared" si="7"/>
-        <v>0.2271</v>
+        <v>0.127</v>
       </c>
       <c r="I14">
         <f t="shared" si="8"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="2"/>
-        <v>Oct</v>
+        <v>Aug</v>
       </c>
       <c r="C15">
         <f t="shared" si="3"/>
-        <v>302100</v>
+        <v>157000</v>
       </c>
       <c r="D15">
         <f t="shared" si="4"/>
-        <v>302.10000000000002</v>
+        <v>157</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F15">
         <f t="shared" si="5"/>
-        <v>105000</v>
+        <v>30000</v>
       </c>
       <c r="G15">
         <f t="shared" si="6"/>
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="H15">
         <f t="shared" si="7"/>
-        <v>0.30210000000000004</v>
+        <v>0.157</v>
       </c>
       <c r="I15">
         <f t="shared" si="8"/>
-        <v>34.700000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="2"/>
-        <v>Nov</v>
+        <v>Sep</v>
       </c>
       <c r="C16">
         <f t="shared" si="3"/>
-        <v>407100</v>
+        <v>187000</v>
       </c>
       <c r="D16">
         <f t="shared" si="4"/>
-        <v>407.1</v>
+        <v>187</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F16">
         <f t="shared" si="5"/>
-        <v>150000</v>
+        <v>40000</v>
       </c>
       <c r="G16">
         <f t="shared" si="6"/>
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="H16">
         <f t="shared" si="7"/>
-        <v>0.40710000000000002</v>
+        <v>0.187</v>
       </c>
       <c r="I16">
         <f t="shared" si="8"/>
-        <v>36.799999999999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="2"/>
-        <v>Dec</v>
+        <v>Oct</v>
       </c>
       <c r="C17">
         <f t="shared" si="3"/>
-        <v>557100</v>
+        <v>227000</v>
       </c>
       <c r="D17">
         <f t="shared" si="4"/>
-        <v>557.1</v>
+        <v>227</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F17">
         <f t="shared" si="5"/>
-        <v>195000</v>
+        <v>50000</v>
       </c>
       <c r="G17">
         <f t="shared" si="6"/>
-        <v>195</v>
+        <v>50</v>
       </c>
       <c r="H17">
         <f t="shared" si="7"/>
-        <v>0.55710000000000004</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="I17">
         <f t="shared" si="8"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
       <c r="B18" t="str">
         <f>TEXT((ROW()-ROW($B$8)+$E$4)*29,"mmm")</f>
-        <v>Jan</v>
+        <v>Nov</v>
       </c>
       <c r="C18">
         <f t="shared" si="3"/>
-        <v>752100</v>
+        <v>277000</v>
       </c>
       <c r="D18">
         <f t="shared" si="4"/>
-        <v>752.1</v>
+        <v>277</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F18">
         <f t="shared" si="5"/>
-        <v>270000</v>
+        <v>60000</v>
       </c>
       <c r="G18">
         <f t="shared" si="6"/>
-        <v>270</v>
+        <v>60</v>
       </c>
       <c r="H18">
         <f t="shared" si="7"/>
-        <v>0.75209999999999999</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="I18">
         <f t="shared" si="8"/>
-        <v>35.799999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" ref="B19:B29" si="9">TEXT((ROW()-ROW($B$8)+$E$4)*29,"mmm")</f>
-        <v>Feb</v>
+        <v>Dec</v>
       </c>
       <c r="C19">
         <f t="shared" si="3"/>
-        <v>1022100</v>
+        <v>337000</v>
       </c>
       <c r="D19">
         <f t="shared" si="4"/>
-        <v>1022.1</v>
+        <v>337</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <f t="shared" si="5"/>
-        <v>375000</v>
+        <v>80000</v>
       </c>
       <c r="G19">
         <f t="shared" si="6"/>
-        <v>375</v>
+        <v>80</v>
       </c>
       <c r="H19">
         <f t="shared" si="7"/>
-        <v>1.0221</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="I19">
         <f t="shared" si="8"/>
-        <v>36.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="9"/>
-        <v>Mar</v>
+        <v>Jan</v>
       </c>
       <c r="C20">
         <f t="shared" si="3"/>
-        <v>1397100</v>
+        <v>417000</v>
       </c>
       <c r="D20">
         <f t="shared" si="4"/>
-        <v>1397.1</v>
+        <v>417</v>
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <f t="shared" si="5"/>
-        <v>510000</v>
+        <v>100000</v>
       </c>
       <c r="G20">
         <f t="shared" si="6"/>
-        <v>510</v>
+        <v>100</v>
       </c>
       <c r="H20">
         <f t="shared" si="7"/>
-        <v>1.3971</v>
+        <v>0.41699999999999998</v>
       </c>
       <c r="I20">
         <f t="shared" si="8"/>
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="9"/>
-        <v>Apr</v>
+        <v>Feb</v>
       </c>
       <c r="C21">
         <f t="shared" si="3"/>
-        <v>1907100</v>
+        <v>517000</v>
       </c>
       <c r="D21">
         <f t="shared" si="4"/>
-        <v>1907.1</v>
+        <v>517</v>
       </c>
       <c r="E21">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F21">
         <f t="shared" si="5"/>
-        <v>705000</v>
+        <v>120000</v>
       </c>
       <c r="G21">
         <f t="shared" si="6"/>
-        <v>705</v>
+        <v>120</v>
       </c>
       <c r="H21">
         <f t="shared" si="7"/>
-        <v>1.9071</v>
+        <v>0.51700000000000002</v>
       </c>
       <c r="I21">
         <f t="shared" si="8"/>
-        <v>36.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="9"/>
-        <v>May</v>
+        <v>Mar</v>
       </c>
       <c r="C22">
         <f t="shared" si="3"/>
-        <v>2612100</v>
+        <v>637000</v>
       </c>
       <c r="D22">
         <f t="shared" si="4"/>
-        <v>2612.1</v>
+        <v>637</v>
       </c>
       <c r="E22">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="F22">
         <f t="shared" si="5"/>
-        <v>975000</v>
+        <v>150000</v>
       </c>
       <c r="G22">
         <f t="shared" si="6"/>
-        <v>975</v>
+        <v>150</v>
       </c>
       <c r="H22">
         <f t="shared" si="7"/>
-        <v>2.6120999999999999</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="I22">
         <f t="shared" si="8"/>
-        <v>37.299999999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="9"/>
-        <v>Jun</v>
+        <v>Apr</v>
       </c>
       <c r="C23">
         <f t="shared" si="3"/>
-        <v>3587100</v>
+        <v>787000</v>
       </c>
       <c r="D23">
         <f t="shared" si="4"/>
-        <v>3587.1</v>
+        <v>787</v>
       </c>
       <c r="E23">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="F23">
         <f t="shared" si="5"/>
-        <v>1335000</v>
+        <v>190000</v>
       </c>
       <c r="G23">
         <f t="shared" si="6"/>
-        <v>1335</v>
+        <v>190</v>
       </c>
       <c r="H23">
         <f t="shared" si="7"/>
-        <v>3.5871</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="I23">
         <f t="shared" si="8"/>
-        <v>37.200000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="9"/>
-        <v>Jul</v>
+        <v>May</v>
       </c>
       <c r="C24">
         <f t="shared" si="3"/>
-        <v>4922100</v>
+        <v>977000</v>
       </c>
       <c r="D24">
         <f t="shared" si="4"/>
-        <v>4922.1000000000004</v>
+        <v>977</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="F24">
         <f t="shared" si="5"/>
-        <v>1845000</v>
+        <v>240000</v>
       </c>
       <c r="G24">
         <f t="shared" si="6"/>
-        <v>1845</v>
+        <v>240</v>
       </c>
       <c r="H24">
         <f t="shared" si="7"/>
-        <v>4.9221000000000004</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="I24">
         <f t="shared" si="8"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="9"/>
-        <v>Aug</v>
+        <v>Jun</v>
       </c>
       <c r="C25">
         <f t="shared" si="3"/>
-        <v>6767100</v>
+        <v>1217000</v>
       </c>
       <c r="D25">
         <f t="shared" si="4"/>
-        <v>6767.1</v>
+        <v>1217</v>
       </c>
       <c r="E25">
         <f t="shared" si="1"/>
-        <v>169</v>
+        <v>30</v>
       </c>
       <c r="F25">
         <f t="shared" si="5"/>
-        <v>2535000</v>
+        <v>300000</v>
       </c>
       <c r="G25">
         <f t="shared" si="6"/>
-        <v>2535</v>
+        <v>300</v>
       </c>
       <c r="H25">
         <f t="shared" si="7"/>
-        <v>6.7671000000000001</v>
+        <v>1.2170000000000001</v>
       </c>
       <c r="I25">
         <f t="shared" si="8"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="9"/>
-        <v>Aug</v>
+        <v>Jul</v>
       </c>
       <c r="C26">
         <f t="shared" si="3"/>
-        <v>9302100</v>
+        <v>1517000</v>
       </c>
       <c r="D26">
         <f t="shared" si="4"/>
-        <v>9302.1</v>
+        <v>1517</v>
       </c>
       <c r="E26">
         <f t="shared" si="1"/>
-        <v>232</v>
+        <v>37</v>
       </c>
       <c r="F26">
         <f t="shared" si="5"/>
-        <v>3480000</v>
+        <v>370000</v>
       </c>
       <c r="G26">
         <f t="shared" si="6"/>
-        <v>3480</v>
+        <v>370</v>
       </c>
       <c r="H26">
         <f t="shared" si="7"/>
-        <v>9.3021000000000011</v>
+        <v>1.5169999999999999</v>
       </c>
       <c r="I26">
         <f t="shared" si="8"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="9"/>
-        <v>Sep</v>
+        <v>Aug</v>
       </c>
       <c r="C27">
         <f t="shared" si="3"/>
-        <v>12782100</v>
+        <v>1887000</v>
       </c>
       <c r="D27">
         <f t="shared" si="4"/>
-        <v>12782.1</v>
+        <v>1887</v>
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>319</v>
+        <v>47</v>
       </c>
       <c r="F27">
         <f t="shared" si="5"/>
-        <v>4785000</v>
+        <v>470000</v>
       </c>
       <c r="G27">
         <f t="shared" si="6"/>
-        <v>4785</v>
+        <v>470</v>
       </c>
       <c r="H27">
         <f t="shared" si="7"/>
-        <v>12.7821</v>
+        <v>1.887</v>
       </c>
       <c r="I27">
         <f t="shared" si="8"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="9"/>
-        <v>Oct</v>
+        <v>Aug</v>
       </c>
       <c r="C28">
         <f t="shared" si="3"/>
-        <v>17567100</v>
+        <v>2357000</v>
       </c>
       <c r="D28">
         <f t="shared" ref="D28:D29" si="10">C28/1000</f>
-        <v>17567.099999999999</v>
+        <v>2357</v>
       </c>
       <c r="E28">
         <f t="shared" si="1"/>
-        <v>439</v>
+        <v>58</v>
       </c>
       <c r="F28">
         <f t="shared" si="5"/>
-        <v>6585000</v>
+        <v>580000</v>
       </c>
       <c r="G28">
         <f t="shared" si="6"/>
-        <v>6585</v>
+        <v>580</v>
       </c>
       <c r="H28">
         <f t="shared" si="7"/>
-        <v>17.5671</v>
+        <v>2.3570000000000002</v>
       </c>
       <c r="I28">
         <f t="shared" si="8"/>
-        <v>37.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="9"/>
-        <v>Nov</v>
+        <v>Sep</v>
       </c>
       <c r="C29">
         <f t="shared" si="3"/>
-        <v>24152100</v>
+        <v>2937000</v>
       </c>
       <c r="D29">
         <f t="shared" si="10"/>
-        <v>24152.1</v>
+        <v>2937</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>603</v>
+        <v>73</v>
       </c>
       <c r="F29">
         <f t="shared" si="5"/>
-        <v>9045000</v>
+        <v>730000</v>
       </c>
       <c r="G29">
         <f t="shared" si="6"/>
-        <v>9045</v>
+        <v>730</v>
       </c>
       <c r="H29">
         <f t="shared" si="7"/>
-        <v>24.152099999999997</v>
+        <v>2.9369999999999998</v>
       </c>
       <c r="I29">
         <f t="shared" si="8"/>
-        <v>37.4</v>
+        <v>24.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>